<commit_message>
Solución de problemas en resoluciones
Se solucionaron los problemas en las resoluciones, respecto a la temporalidad.
</commit_message>
<xml_diff>
--- a/format/medidasDeProteccion/documents/GeneratedFile.xlsx
+++ b/format/medidasDeProteccion/documents/GeneratedFile.xlsx
@@ -15,12 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="69">
-  <si>
-    <t>Periodo Correspondiente: 12-2024</t>
-  </si>
-  <si>
-    <t>Consultado: 06-12-2024</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="68">
+  <si>
+    <t>Periodo Correspondiente: 2-12-2024</t>
+  </si>
+  <si>
+    <t>Consultado: 11-12-2024</t>
   </si>
   <si>
     <t>Información Obtenida del Sistema Integral de Registro Estadístico (SIRE)</t>
@@ -80,6 +80,9 @@
     <t>Ampliación</t>
   </si>
   <si>
+    <t>Coorporación Policial</t>
+  </si>
+  <si>
     <t>I</t>
   </si>
   <si>
@@ -116,17 +119,17 @@
     <t>No</t>
   </si>
   <si>
-    <t>Prueba Prueba Prueba</t>
-  </si>
-  <si>
-    <t>1003202400051</t>
-  </si>
-  <si>
-    <t>Homicidio doloso</t>
+    <t>Javier Andres Bucio García</t>
+  </si>
+  <si>
+    <t>1007202445929</t>
+  </si>
+  <si>
+    <t>Amenazas</t>
   </si>
   <si>
     <t xml:space="preserve">
-Juan Pérez Maldonado</t>
+IVAN MORA ROJAS</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -134,7 +137,7 @@
   </si>
   <si>
     <t xml:space="preserve">
-21</t>
+49</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -142,90 +145,53 @@
   </si>
   <si>
     <t xml:space="preserve">
-Baja California Sur</t>
+Michoacán de Ocampo</t>
   </si>
   <si>
     <t xml:space="preserve">
-Comondú</t>
+Yurécuaro</t>
   </si>
   <si>
     <t xml:space="preserve">
-Prohibición de acercarse o comunicarse con la víctima u ofendido
-Vigilancia en el domicilio de la víctima u ofendido</t>
-  </si>
-  <si>
-    <t>2024-12-06 13:35:53</t>
-  </si>
-  <si>
-    <t>2024-12-05 13:34:00</t>
-  </si>
-  <si>
-    <t>2024-12-06 13:42:00</t>
+La prohibición de realizar conductas de intimidación o molestia a la víctima u ofendido o a personas relacionados con ellos
+Vigilancia en el domicilio de la víctima u ofendido
+Protección policial de la víctima u ofendido
+Auxilio inmediato por integrantes de instituciones policiales, al domicilio en donde se localice o se encuentre la víctima u ofendido en el momento de solicitarlo
+Traslado de la víctima u ofendido a refugios o albergues temporales, así como de sus descendientes
+El reingreso de la víctima u ofendido a su domicilio, una vez que se salvaguarde su seguridad</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>2024-12-10 20:31:18</t>
+  </si>
+  <si>
+    <t>2024-12-02 13:00:00</t>
+  </si>
+  <si>
+    <t>2025-02-02 13:00:00</t>
+  </si>
+  <si>
+    <t>Brenda Lisset Jaimes Arroyo</t>
+  </si>
+  <si>
+    <t>1003202445885</t>
+  </si>
+  <si>
+    <t>Lesiones en razón de parentesco o relación</t>
   </si>
   <si>
     <t xml:space="preserve">
-Juan Pérez Arriaga</t>
+GABRIELA MORENO HERNANDEZ</t>
   </si>
   <si>
     <t xml:space="preserve">
-Baja California</t>
+Femenino</t>
   </si>
   <si>
     <t xml:space="preserve">
-Ensenada</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Vigilancia en el domicilio de la víctima u ofendido
-Protección policial de la víctima u ofendido</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>2024-12-05 12:23:09</t>
-  </si>
-  <si>
-    <t>2024-12-05 12:03:00</t>
-  </si>
-  <si>
-    <t>2025-01-25 07:03:00</t>
-  </si>
-  <si>
-    <t>Homicidio en razon de la preferencia sexual</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Carlos Vanegas Campos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Limitación para asistir o acercarse al domicilio de la víctima u ofendido o al lugar donde se encuentre
-Vigilancia en el domicilio de la víctima u ofendido</t>
-  </si>
-  <si>
-    <t>2024-12-05 10:32:48</t>
-  </si>
-  <si>
-    <t>2024-12-04 10:31:00</t>
-  </si>
-  <si>
-    <t>2025-01-10 16:31:00</t>
-  </si>
-  <si>
-    <t>Lesiones culposas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Juan Chiquito Pérez</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-39</t>
+31</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -233,17 +199,50 @@
   </si>
   <si>
     <t xml:space="preserve">
+La prohibición de realizar conductas de intimidación o molestia a la víctima u ofendido o a personas relacionados con ellos
+Vigilancia en el domicilio de la víctima u ofendido
 Protección policial de la víctima u ofendido
 Auxilio inmediato por integrantes de instituciones policiales, al domicilio en donde se localice o se encuentre la víctima u ofendido en el momento de solicitarlo</t>
   </si>
   <si>
-    <t>2024-12-02 14:01:57</t>
-  </si>
-  <si>
-    <t>2024-12-01 14:01:00</t>
-  </si>
-  <si>
-    <t>2024-12-31 14:01:00</t>
+    <t>2024-12-09 15:38:12</t>
+  </si>
+  <si>
+    <t>2024-12-02 12:00:00</t>
+  </si>
+  <si>
+    <t>2025-01-01 12:00:00</t>
+  </si>
+  <si>
+    <t>1003202446007</t>
+  </si>
+  <si>
+    <t>Violencia familiar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+MERITH LILIANA FLORES PARDO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+37</t>
+  </si>
+  <si>
+    <t>2024-12-09 15:34:49</t>
+  </si>
+  <si>
+    <t>1003202446054</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+PATRICIA GONZALEZ HERNANDEZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+25</t>
+  </si>
+  <si>
+    <t>2024-12-09 15:32:18</t>
   </si>
 </sst>
 </file>
@@ -364,6 +363,27 @@
       </bottom>
     </border>
     <border>
+      <right style="thin">
+        <color rgb="152f4a"/>
+      </right>
+      <top style="thin">
+        <color rgb="152f4a"/>
+      </top>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="152f4a"/>
+      </right>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="152f4a"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="152f4a"/>
+      </bottom>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
@@ -433,6 +453,11 @@
       </top>
     </border>
     <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="152f4a"/>
       </left>
@@ -452,32 +477,6 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="152f4a"/>
-      </right>
-      <top style="thin">
-        <color rgb="152f4a"/>
-      </top>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="152f4a"/>
-      </right>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="152f4a"/>
-      </right>
-      <bottom style="thin">
-        <color rgb="152f4a"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
     </border>
     <border>
       <right style="thin">
@@ -513,40 +512,58 @@
     <xf xfId="0" fontId="2" numFmtId="0" fillId="3" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="3" borderId="6" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="3" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="3" borderId="8" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
     <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="6" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="8" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="9" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="10" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="11" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="11" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="12" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="4" numFmtId="0" fillId="3" borderId="12" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="13" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="14" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="15" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="3" borderId="16" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="4" borderId="8" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="4" borderId="11" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="3" numFmtId="0" fillId="4" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="4" borderId="13" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="4" borderId="15" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="4" borderId="14" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="4" borderId="17" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="4" borderId="18" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="4" borderId="19" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
@@ -555,37 +572,19 @@
     <xf xfId="0" fontId="2" numFmtId="0" fillId="3" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="3" borderId="15" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="3" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="3" borderId="16" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="3" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="3" borderId="17" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
     <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="18" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
     <xf xfId="0" fontId="3" numFmtId="0" fillId="4" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="3" numFmtId="0" fillId="4" borderId="18" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="4" borderId="14" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="4" borderId="19" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -631,7 +630,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>24</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -982,7 +981,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AC14"/>
+  <dimension ref="A1:AD14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="AC14" sqref="AC14"/>
@@ -1019,133 +1018,138 @@
     <col min="27" max="27" width="6.75" customWidth="true" style="0"/>
     <col min="28" max="28" width="6.75" customWidth="true" style="0"/>
     <col min="29" max="29" width="17.85" customWidth="true" style="0"/>
+    <col min="30" max="30" width="27" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:30">
       <c r="A1" s="2"/>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
-      <c r="G1" s="20"/>
+      <c r="G1" s="26"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
-      <c r="K1" s="20"/>
+      <c r="K1" s="26"/>
       <c r="L1" s="4"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
-      <c r="T1" s="20"/>
-      <c r="U1" s="20"/>
-      <c r="V1" s="20"/>
-      <c r="W1" s="20"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
       <c r="X1" s="4"/>
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
-      <c r="AA1" s="20"/>
-      <c r="AB1" s="20"/>
-      <c r="AC1" s="21"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="7"/>
     </row>
-    <row r="2" spans="1:29">
+    <row r="2" spans="1:30">
       <c r="A2" s="3"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="22"/>
+      <c r="G2" s="27"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
-      <c r="K2" s="22"/>
+      <c r="K2" s="27"/>
       <c r="L2" s="5"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
-      <c r="S2" s="22"/>
-      <c r="T2" s="22"/>
-      <c r="U2" s="22"/>
-      <c r="V2" s="22"/>
-      <c r="W2" s="22"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="27"/>
+      <c r="R2" s="27"/>
+      <c r="S2" s="27"/>
+      <c r="T2" s="27"/>
+      <c r="U2" s="27"/>
+      <c r="V2" s="27"/>
+      <c r="W2" s="27"/>
       <c r="X2" s="5"/>
       <c r="Y2" s="5"/>
       <c r="Z2" s="5"/>
-      <c r="AA2" s="22"/>
-      <c r="AB2" s="22"/>
-      <c r="AC2" s="23"/>
+      <c r="AA2" s="27"/>
+      <c r="AB2" s="27"/>
+      <c r="AC2" s="27"/>
+      <c r="AD2" s="8"/>
     </row>
-    <row r="3" spans="1:29">
+    <row r="3" spans="1:30">
       <c r="A3" s="3"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
-      <c r="G3" s="22"/>
+      <c r="G3" s="27"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
-      <c r="K3" s="22"/>
+      <c r="K3" s="27"/>
       <c r="L3" s="5"/>
-      <c r="M3" s="22"/>
-      <c r="N3" s="22"/>
-      <c r="O3" s="22"/>
-      <c r="P3" s="22"/>
-      <c r="Q3" s="22"/>
-      <c r="R3" s="22"/>
-      <c r="S3" s="22"/>
-      <c r="T3" s="22"/>
-      <c r="U3" s="22"/>
-      <c r="V3" s="22"/>
-      <c r="W3" s="22"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="27"/>
+      <c r="O3" s="27"/>
+      <c r="P3" s="27"/>
+      <c r="Q3" s="27"/>
+      <c r="R3" s="27"/>
+      <c r="S3" s="27"/>
+      <c r="T3" s="27"/>
+      <c r="U3" s="27"/>
+      <c r="V3" s="27"/>
+      <c r="W3" s="27"/>
       <c r="X3" s="5"/>
       <c r="Y3" s="5"/>
       <c r="Z3" s="5"/>
-      <c r="AA3" s="22"/>
-      <c r="AB3" s="22"/>
-      <c r="AC3" s="23"/>
+      <c r="AA3" s="27"/>
+      <c r="AB3" s="27"/>
+      <c r="AC3" s="27"/>
+      <c r="AD3" s="8"/>
     </row>
-    <row r="4" spans="1:29">
+    <row r="4" spans="1:30">
       <c r="A4" s="3"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
-      <c r="G4" s="22"/>
+      <c r="G4" s="27"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
-      <c r="K4" s="22"/>
+      <c r="K4" s="27"/>
       <c r="L4" s="5"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="22"/>
-      <c r="O4" s="22"/>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="22"/>
-      <c r="S4" s="22"/>
-      <c r="T4" s="22"/>
-      <c r="U4" s="22"/>
-      <c r="V4" s="22"/>
-      <c r="W4" s="22"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="27"/>
+      <c r="O4" s="27"/>
+      <c r="P4" s="27"/>
+      <c r="Q4" s="27"/>
+      <c r="R4" s="27"/>
+      <c r="S4" s="27"/>
+      <c r="T4" s="27"/>
+      <c r="U4" s="27"/>
+      <c r="V4" s="27"/>
+      <c r="W4" s="27"/>
       <c r="X4" s="5"/>
       <c r="Y4" s="5"/>
       <c r="Z4" s="5"/>
-      <c r="AA4" s="22"/>
-      <c r="AB4" s="22"/>
-      <c r="AC4" s="23"/>
+      <c r="AA4" s="27"/>
+      <c r="AB4" s="27"/>
+      <c r="AC4" s="27"/>
+      <c r="AD4" s="8"/>
     </row>
-    <row r="5" spans="1:29">
+    <row r="5" spans="1:30">
       <c r="A5" s="3"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5" t="s">
@@ -1154,31 +1158,32 @@
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="22"/>
+      <c r="G5" s="27"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="22"/>
+      <c r="K5" s="27"/>
       <c r="L5" s="5"/>
-      <c r="M5" s="22"/>
-      <c r="N5" s="22"/>
-      <c r="O5" s="22"/>
-      <c r="P5" s="22"/>
-      <c r="Q5" s="22"/>
-      <c r="R5" s="22"/>
-      <c r="S5" s="22"/>
-      <c r="T5" s="22"/>
-      <c r="U5" s="22"/>
-      <c r="V5" s="22"/>
-      <c r="W5" s="22"/>
+      <c r="M5" s="27"/>
+      <c r="N5" s="27"/>
+      <c r="O5" s="27"/>
+      <c r="P5" s="27"/>
+      <c r="Q5" s="27"/>
+      <c r="R5" s="27"/>
+      <c r="S5" s="27"/>
+      <c r="T5" s="27"/>
+      <c r="U5" s="27"/>
+      <c r="V5" s="27"/>
+      <c r="W5" s="27"/>
       <c r="X5" s="5"/>
       <c r="Y5" s="5"/>
       <c r="Z5" s="5"/>
-      <c r="AA5" s="22"/>
-      <c r="AB5" s="22"/>
-      <c r="AC5" s="23"/>
+      <c r="AA5" s="27"/>
+      <c r="AB5" s="27"/>
+      <c r="AC5" s="27"/>
+      <c r="AD5" s="8"/>
     </row>
-    <row r="6" spans="1:29">
+    <row r="6" spans="1:30">
       <c r="A6" s="3"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5" t="s">
@@ -1187,63 +1192,65 @@
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="22"/>
+      <c r="G6" s="27"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
-      <c r="K6" s="22"/>
+      <c r="K6" s="27"/>
       <c r="L6" s="5"/>
-      <c r="M6" s="22"/>
-      <c r="N6" s="22"/>
-      <c r="O6" s="22"/>
-      <c r="P6" s="22"/>
-      <c r="Q6" s="22"/>
-      <c r="R6" s="22"/>
-      <c r="S6" s="22"/>
-      <c r="T6" s="22"/>
-      <c r="U6" s="22"/>
-      <c r="V6" s="22"/>
-      <c r="W6" s="22"/>
+      <c r="M6" s="27"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="27"/>
+      <c r="P6" s="27"/>
+      <c r="Q6" s="27"/>
+      <c r="R6" s="27"/>
+      <c r="S6" s="27"/>
+      <c r="T6" s="27"/>
+      <c r="U6" s="27"/>
+      <c r="V6" s="27"/>
+      <c r="W6" s="27"/>
       <c r="X6" s="5"/>
       <c r="Y6" s="5"/>
       <c r="Z6" s="5"/>
-      <c r="AA6" s="22"/>
-      <c r="AB6" s="22"/>
-      <c r="AC6" s="23"/>
+      <c r="AA6" s="27"/>
+      <c r="AB6" s="27"/>
+      <c r="AC6" s="27"/>
+      <c r="AD6" s="8"/>
     </row>
-    <row r="7" spans="1:29">
+    <row r="7" spans="1:30">
       <c r="A7" s="3"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="22"/>
+      <c r="G7" s="27"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
-      <c r="K7" s="22"/>
+      <c r="K7" s="27"/>
       <c r="L7" s="5"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="22"/>
-      <c r="O7" s="22"/>
-      <c r="P7" s="22"/>
-      <c r="Q7" s="22"/>
-      <c r="R7" s="22"/>
-      <c r="S7" s="22"/>
-      <c r="T7" s="22"/>
-      <c r="U7" s="22"/>
-      <c r="V7" s="22"/>
-      <c r="W7" s="22"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="27"/>
+      <c r="O7" s="27"/>
+      <c r="P7" s="27"/>
+      <c r="Q7" s="27"/>
+      <c r="R7" s="27"/>
+      <c r="S7" s="27"/>
+      <c r="T7" s="27"/>
+      <c r="U7" s="27"/>
+      <c r="V7" s="27"/>
+      <c r="W7" s="27"/>
       <c r="X7" s="5"/>
       <c r="Y7" s="5"/>
       <c r="Z7" s="5"/>
-      <c r="AA7" s="22"/>
-      <c r="AB7" s="22"/>
-      <c r="AC7" s="23"/>
+      <c r="AA7" s="27"/>
+      <c r="AB7" s="27"/>
+      <c r="AC7" s="27"/>
+      <c r="AD7" s="8"/>
     </row>
-    <row r="8" spans="1:29">
-      <c r="A8" s="14"/>
+    <row r="8" spans="1:30">
+      <c r="A8" s="18"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6" t="s">
         <v>2</v>
@@ -1251,101 +1258,105 @@
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
-      <c r="G8" s="24"/>
+      <c r="G8" s="28"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
-      <c r="K8" s="24"/>
+      <c r="K8" s="28"/>
       <c r="L8" s="6"/>
-      <c r="M8" s="24"/>
-      <c r="N8" s="24"/>
-      <c r="O8" s="24"/>
-      <c r="P8" s="24"/>
-      <c r="Q8" s="24"/>
-      <c r="R8" s="24"/>
-      <c r="S8" s="24"/>
-      <c r="T8" s="24"/>
-      <c r="U8" s="24"/>
-      <c r="V8" s="24"/>
-      <c r="W8" s="24"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="28"/>
+      <c r="R8" s="28"/>
+      <c r="S8" s="28"/>
+      <c r="T8" s="28"/>
+      <c r="U8" s="28"/>
+      <c r="V8" s="28"/>
+      <c r="W8" s="28"/>
       <c r="X8" s="6"/>
       <c r="Y8" s="6"/>
       <c r="Z8" s="6"/>
-      <c r="AA8" s="24"/>
-      <c r="AB8" s="24"/>
-      <c r="AC8" s="25"/>
+      <c r="AA8" s="28"/>
+      <c r="AB8" s="28"/>
+      <c r="AC8" s="28"/>
+      <c r="AD8" s="9"/>
     </row>
-    <row r="9" spans="1:29">
-      <c r="A9" s="8" t="s">
+    <row r="9" spans="1:30">
+      <c r="A9" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="I9" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="J9" s="11" t="s">
+      <c r="J9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="K9" s="11" t="s">
+      <c r="K9" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="L9" s="11" t="s">
+      <c r="L9" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="M9" s="11" t="s">
+      <c r="M9" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11"/>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="11"/>
-      <c r="R9" s="11"/>
-      <c r="S9" s="11"/>
-      <c r="T9" s="11"/>
-      <c r="U9" s="11"/>
-      <c r="V9" s="11"/>
-      <c r="W9" s="11" t="s">
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="14"/>
+      <c r="T9" s="14"/>
+      <c r="U9" s="14"/>
+      <c r="V9" s="14"/>
+      <c r="W9" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="X9" s="11" t="s">
+      <c r="X9" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="Y9" s="11" t="s">
+      <c r="Y9" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="Z9" s="11" t="s">
+      <c r="Z9" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="AA9" s="11" t="s">
+      <c r="AA9" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="AB9" s="11"/>
-      <c r="AC9" s="12" t="s">
+      <c r="AB9" s="14"/>
+      <c r="AC9" s="14" t="s">
         <v>16</v>
       </c>
+      <c r="AD9" s="15" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="10" spans="1:29">
-      <c r="A10" s="9"/>
+    <row r="10" spans="1:30">
+      <c r="A10" s="12"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -1358,334 +1369,355 @@
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="V10" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="W10" s="1"/>
       <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
       <c r="AA10" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AB10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC10" s="13"/>
+        <v>33</v>
+      </c>
+      <c r="AC10" s="1"/>
+      <c r="AD10" s="16"/>
     </row>
-    <row r="11" spans="1:29">
-      <c r="A11" s="10">
-        <v>4829</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="7" t="s">
+    <row r="11" spans="1:30">
+      <c r="A11" s="13">
+        <v>4970</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="C11" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="D11" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="E11" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="G11" s="26" t="s">
+      <c r="F11" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="G11" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="H11" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="J11" s="7" t="s">
+      <c r="I11" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="K11" s="26">
-        <v>2</v>
-      </c>
-      <c r="L11" s="7" t="s">
+      <c r="J11" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="M11" s="26" t="s">
+      <c r="K11" s="29">
+        <v>6</v>
+      </c>
+      <c r="L11" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="M11" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="N11" s="29"/>
+      <c r="O11" s="29"/>
+      <c r="P11" s="29"/>
+      <c r="Q11" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="R11" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="S11" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="T11" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="U11" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="V11" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="W11" s="29">
+        <v>62</v>
+      </c>
+      <c r="X11" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y11" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z11" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA11" s="29"/>
+      <c r="AB11" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC11" s="29"/>
+      <c r="AD11" s="17"/>
+    </row>
+    <row r="12" spans="1:30">
+      <c r="A12" s="19">
+        <v>4889</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="I12" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="J12" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="K12" s="30">
+        <v>4</v>
+      </c>
+      <c r="L12" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="M12" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="N12" s="30"/>
+      <c r="O12" s="30"/>
+      <c r="P12" s="30"/>
+      <c r="Q12" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="R12" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="S12" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="T12" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="U12" s="30"/>
+      <c r="V12" s="30"/>
+      <c r="W12" s="30">
         <v>30</v>
       </c>
-      <c r="N11" s="26"/>
-      <c r="O11" s="26"/>
-      <c r="P11" s="26"/>
-      <c r="Q11" s="26"/>
-      <c r="R11" s="26" t="s">
+      <c r="X12" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y12" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z12" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA12" s="30"/>
+      <c r="AB12" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC12" s="30"/>
+      <c r="AD12" s="21"/>
+    </row>
+    <row r="13" spans="1:30">
+      <c r="A13" s="13">
+        <v>4888</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="K13" s="29">
+        <v>4</v>
+      </c>
+      <c r="L13" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="M13" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="N13" s="29"/>
+      <c r="O13" s="29"/>
+      <c r="P13" s="29"/>
+      <c r="Q13" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="R13" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="S13" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="T13" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="U13" s="29"/>
+      <c r="V13" s="29"/>
+      <c r="W13" s="29">
         <v>30</v>
       </c>
-      <c r="S11" s="26"/>
-      <c r="T11" s="26"/>
-      <c r="U11" s="26"/>
-      <c r="V11" s="26"/>
-      <c r="W11" s="26">
-        <v>25</v>
-      </c>
-      <c r="X11" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y11" s="7" t="s">
+      <c r="X13" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y13" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z13" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA13" s="29"/>
+      <c r="AB13" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC13" s="29"/>
+      <c r="AD13" s="17"/>
+    </row>
+    <row r="14" spans="1:30">
+      <c r="A14" s="22">
+        <v>4887</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="H14" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="I14" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="J14" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="K14" s="31">
+        <v>4</v>
+      </c>
+      <c r="L14" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="M14" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="Z11" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA11" s="26" t="s">
+      <c r="N14" s="31"/>
+      <c r="O14" s="31"/>
+      <c r="P14" s="31"/>
+      <c r="Q14" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="R14" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="S14" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="T14" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="U14" s="31"/>
+      <c r="V14" s="31"/>
+      <c r="W14" s="31">
         <v>30</v>
       </c>
-      <c r="AB11" s="26"/>
-      <c r="AC11" s="27">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:29">
-      <c r="A12" s="15">
-        <v>4827</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="G12" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="H12" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="I12" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="J12" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="K12" s="28">
-        <v>2</v>
-      </c>
-      <c r="L12" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="M12" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="N12" s="28"/>
-      <c r="O12" s="28"/>
-      <c r="P12" s="28"/>
-      <c r="Q12" s="28"/>
-      <c r="R12" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="S12" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="T12" s="28"/>
-      <c r="U12" s="28"/>
-      <c r="V12" s="28"/>
-      <c r="W12" s="28">
-        <v>10</v>
-      </c>
-      <c r="X12" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y12" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="Z12" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="AA12" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="AB12" s="28"/>
-      <c r="AC12" s="29">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:29">
-      <c r="A13" s="10">
-        <v>4826</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="G13" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="J13" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="K13" s="26">
-        <v>2</v>
-      </c>
-      <c r="L13" s="7" t="s">
+      <c r="X14" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y14" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="M13" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="N13" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="O13" s="26"/>
-      <c r="P13" s="26"/>
-      <c r="Q13" s="26"/>
-      <c r="R13" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="S13" s="26"/>
-      <c r="T13" s="26"/>
-      <c r="U13" s="26"/>
-      <c r="V13" s="26"/>
-      <c r="W13" s="26">
-        <v>26</v>
-      </c>
-      <c r="X13" s="7" t="s">
+      <c r="Z14" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="Y13" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="Z13" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AA13" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="AB13" s="26"/>
-      <c r="AC13" s="27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:29">
-      <c r="A14" s="17">
-        <v>4825</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="F14" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="G14" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="H14" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="I14" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="J14" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="K14" s="30">
-        <v>2</v>
-      </c>
-      <c r="L14" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="M14" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="N14" s="30"/>
-      <c r="O14" s="30"/>
-      <c r="P14" s="30"/>
-      <c r="Q14" s="30"/>
-      <c r="R14" s="30"/>
-      <c r="S14" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="T14" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="U14" s="30"/>
-      <c r="V14" s="30"/>
-      <c r="W14" s="30">
-        <v>30</v>
-      </c>
-      <c r="X14" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="Y14" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="Z14" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA14" s="30"/>
-      <c r="AB14" s="30" t="s">
-        <v>30</v>
+      <c r="AA14" s="31"/>
+      <c r="AB14" s="31" t="s">
+        <v>31</v>
       </c>
       <c r="AC14" s="31"/>
+      <c r="AD14" s="24"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
@@ -1714,6 +1746,7 @@
     <mergeCell ref="X1:AC7"/>
     <mergeCell ref="C5:I5"/>
     <mergeCell ref="C6:I6"/>
+    <mergeCell ref="AD9:AD10"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>